<commit_message>
✨ add generic Oncho file.
</commit_message>
<xml_diff>
--- a/ONCHO/black flies capture/oncho_1_site.xlsx
+++ b/ONCHO/black flies capture/oncho_1_site.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbandubad\Repositories\generic-espen-collect-form\ONCHO\black flies capture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\generic-espen-collect-form\ONCHO\black flies capture\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F519319-BCA2-450E-9C04-2B333E74CAA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="25785" windowHeight="13980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="110">
   <si>
     <t>form_title</t>
   </si>
@@ -130,9 +131,6 @@
     <t>geopoint</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -166,9 +164,6 @@
     <t>yesNoDontKnow</t>
   </si>
   <si>
-    <t>select_one yesNoDontKnow</t>
-  </si>
-  <si>
     <t>1. Black Flies Capture - Site</t>
   </si>
   <si>
@@ -199,9 +194,6 @@
     <t>Name of river or stream</t>
   </si>
   <si>
-    <t>s_river_basin</t>
-  </si>
-  <si>
     <t>Name of river basin</t>
   </si>
   <si>
@@ -317,13 +309,64 @@
   </si>
   <si>
     <t>basin_list</t>
+  </si>
+  <si>
+    <t>stream_list</t>
+  </si>
+  <si>
+    <t>select_one basin_list</t>
+  </si>
+  <si>
+    <t>s_river_basin_name</t>
+  </si>
+  <si>
+    <t>select_one stream_list</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>s_start</t>
+  </si>
+  <si>
+    <t>s_end</t>
+  </si>
+  <si>
+    <t>basin_list=${s_river_basin_name}</t>
+  </si>
+  <si>
+    <t>select_one region_list</t>
+  </si>
+  <si>
+    <t>s_province</t>
+  </si>
+  <si>
+    <t>Select Province</t>
+  </si>
+  <si>
+    <t>Sélectionner une province</t>
+  </si>
+  <si>
+    <t>region_list</t>
+  </si>
+  <si>
+    <t>Region1</t>
+  </si>
+  <si>
+    <t>Region2</t>
+  </si>
+  <si>
+    <t>region_list=${s_province}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -384,6 +427,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -434,7 +483,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -512,6 +561,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -800,36 +850,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:XFD5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.25" customWidth="1"/>
-    <col min="5" max="5" width="47.5" customWidth="1"/>
-    <col min="6" max="6" width="47.375" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.609375" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.5" customWidth="1"/>
-    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="13" max="13" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.875" customWidth="1"/>
-    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.38671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.609375" customWidth="1"/>
+    <col min="13" max="13" width="9.71875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.88671875" customWidth="1"/>
+    <col min="15" max="15" width="28.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
@@ -876,275 +926,286 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="15"/>
       <c r="L2" s="15"/>
       <c r="M2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="14" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="12"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" s="15"/>
-      <c r="O3" s="16"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="17"/>
-      <c r="H4" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="10"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="15"/>
       <c r="M4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N4" s="15"/>
-      <c r="O4" s="16"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="15"/>
+      <c r="B5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="10"/>
       <c r="L5" s="15"/>
       <c r="M5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>54</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6" s="19"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="10"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="15"/>
       <c r="M6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="15"/>
-      <c r="O6" s="16"/>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="15"/>
+        <v>96</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="19"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="15"/>
       <c r="M7" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-    </row>
-    <row r="8" spans="1:15" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="O7" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+    </row>
+    <row r="9" spans="1:15" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C10" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-    </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-    </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>66</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F10" s="24"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="23"/>
+        <v>33</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
+      <c r="E11" s="24" t="s">
+        <v>72</v>
+      </c>
       <c r="F11" s="24"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1156,11 +1217,13 @@
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>99</v>
+      </c>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
@@ -1175,26 +1238,47 @@
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
+    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1203,24 +1287,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.38671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.609375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.71875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.38671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -1233,234 +1318,317 @@
       <c r="D1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
+      <c r="E1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>107</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="29"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="E6" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="E10" s="16"/>
+      <c r="F10" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7" t="s">
+      <c r="E11" s="16"/>
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="E12" s="16"/>
+      <c r="F12" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
+      <c r="E13" s="16"/>
+      <c r="F13" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C14" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="E14" s="16"/>
+      <c r="F14" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="7" t="s">
+      <c r="E15" s="16"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A14:C59">
-    <sortCondition ref="B14:B59"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:C61">
+    <sortCondition ref="B16:B61"/>
   </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="44.125" customWidth="1"/>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.38671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1474,12 +1642,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>20200601</v>

</xml_diff>